<commit_message>
- Alteração slide Dynasys - Bookmark adicionado na planilha para Dynasys - Pasta asset para armazenar imagens
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3_light_version.xlsx
+++ b/Test Enviroment Plan V3_light_version.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T966104\Documents\repos\docs\syngenta-appmap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luciano.daher\Desktop\Syngenta\compart\syngenta-appmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1075,7 +1075,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
refactoring in the integration type enum, changed to another sheet
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3_light_version.xlsx
+++ b/Test Enviroment Plan V3_light_version.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Integration Type</t>
   </si>
@@ -214,43 +214,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$K$2:$K$18" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$L$2:$L$18" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$L$2:$L$18" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$K$2:$K$18" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$L$2:$L$18" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$K$2:$K$18" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$K$2:$K$18" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$L$2:$L$18" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$L$2:$L$18" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="$K$2:$K$18" noThreeD="1" sel="6" val="3"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="6" val="3"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1072,10 +1072,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1092,7 @@
     <col min="12" max="12" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1137,57 +1137,28 @@
       <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
-      </c>
-      <c r="K6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K7" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new links to excel / new integration types
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3_light_version.xlsx
+++ b/Test Enviroment Plan V3_light_version.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Integration Type</t>
   </si>
@@ -106,6 +106,30 @@
   </si>
   <si>
     <t>Flat File / RFC</t>
+  </si>
+  <si>
+    <t>https://www.kewilltransport.net</t>
+  </si>
+  <si>
+    <t>https://cte.kewilltransport.net</t>
+  </si>
+  <si>
+    <t>Ezequias Prado</t>
+  </si>
+  <si>
+    <t>Web Service</t>
+  </si>
+  <si>
+    <t>FTP</t>
+  </si>
+  <si>
+    <t>JDBC</t>
+  </si>
+  <si>
+    <t>Web Service / FTP</t>
+  </si>
+  <si>
+    <t>Carrier Web Services</t>
   </si>
 </sst>
 </file>
@@ -136,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,8 +173,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -184,11 +214,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -196,6 +241,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,6 +269,14 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="2" val="0"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="10" val="5"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="4"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="1" val="0"/>
 </file>
@@ -238,7 +294,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="7" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -246,11 +302,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$C1:$C$18" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="6" val="3"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="16" fmlaRange="'Integration Type'!$A1:$A$18" noThreeD="1" sel="6" val="5"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -805,6 +861,106 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1047750" cy="180975"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Drop Down 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1066800" cy="171450"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1040" name="Drop Down 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1040"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1072,10 +1228,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1240,7 @@
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.85546875" bestFit="1" customWidth="1"/>
@@ -1155,10 +1311,27 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
+      <c r="D5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1389,6 +1562,50 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1039" r:id="rId14" name="Drop Down 15">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1040" r:id="rId15" name="Drop Down 16">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
@@ -1397,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,6 +1654,9 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1446,6 +1666,26 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gitignore para arquivos temp do office
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3_light_version.xlsx
+++ b/Test Enviroment Plan V3_light_version.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="52">
   <si>
     <t>Integration Type</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Application Type</t>
   </si>
   <si>
-    <t>ASM</t>
-  </si>
-  <si>
     <t>Application Name</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Nutrade</t>
   </si>
   <si>
-    <t>Marcela Simioni</t>
-  </si>
-  <si>
     <t>Feed System</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>https://cte.kewilltransport.net</t>
   </si>
   <si>
-    <t>Ezequias Prado</t>
-  </si>
-  <si>
     <t>Web Service</t>
   </si>
   <si>
@@ -189,10 +180,7 @@
     <t>brspwprojdb01</t>
   </si>
   <si>
-    <t xml:space="preserve">Elaine Santos </t>
-  </si>
-  <si>
-    <t>marcela Simioni</t>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -216,7 +204,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -292,25 +282,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -326,8 +304,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -607,401 +595,571 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="E11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="E13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="E17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="E18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="H8" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H11" r:id="rId10"/>
+    <hyperlink ref="H12" r:id="rId11"/>
+    <hyperlink ref="H13" r:id="rId12"/>
+    <hyperlink ref="H14" r:id="rId13"/>
+    <hyperlink ref="H15" r:id="rId14"/>
+    <hyperlink ref="H16" r:id="rId15"/>
+    <hyperlink ref="H17" r:id="rId16"/>
+    <hyperlink ref="H18" r:id="rId17"/>
+    <hyperlink ref="H19" r:id="rId18"/>
+    <hyperlink ref="H20" r:id="rId19"/>
+    <hyperlink ref="H21" r:id="rId20"/>
+    <hyperlink ref="H22" r:id="rId21"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1009,13 +1167,13 @@
           <x14:formula1>
             <xm:f>'Integration Type'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B23</xm:sqref>
+          <xm:sqref>B2:B22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Integration Type'!$C:$C</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C23</xm:sqref>
+          <xm:sqref>C2:C22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1039,72 +1197,72 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes no fluxo as is
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3_light_version.xlsx
+++ b/Test Enviroment Plan V3_light_version.xlsx
@@ -619,8 +619,8 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G14" sqref="G14"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
alterações feitas minutos antes da apresentação
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3_light_version.xlsx
+++ b/Test Enviroment Plan V3_light_version.xlsx
@@ -735,9 +735,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H24" sqref="H24"/>
+      <selection pane="topRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
       </c>
       <c r="H3" s="19"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
versão para o cheng validar
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3_light_version.xlsx
+++ b/Test Enviroment Plan V3_light_version.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="73">
   <si>
     <t>Integration Type</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>W:\SAP_Interfaces\WMAP\Integração com Nutrace</t>
+  </si>
+  <si>
+    <t>ieaziwappd002</t>
+  </si>
+  <si>
+    <t>IEAZIWSQLD001 (10.63.252.71)</t>
   </si>
 </sst>
 </file>
@@ -299,7 +305,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,18 +321,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,13 +379,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -400,55 +391,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -735,9 +704,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,549 +724,549 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="19"/>
-    </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="E3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="15" t="s">
+      <c r="G4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="G5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="16" t="s">
+      <c r="E6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:8" s="8" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="11">
         <v>147167169205</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="16" t="s">
+      <c r="D10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="16" t="s">
+      <c r="D11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="16" t="s">
+      <c r="D12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="24" t="s">
+      <c r="D13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="D14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="D15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="13" t="s">
+      <c r="D16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="13" t="s">
+      <c r="D17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="D18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="10" t="s">
+      <c r="B20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="B21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="24"/>
+      <c r="B22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ultima versão enviada ao cheng
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3_light_version.xlsx
+++ b/Test Enviroment Plan V3_light_version.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="75">
   <si>
     <t>Integration Type</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>CR + timestamp / CRBaixa + timestamp</t>
-  </si>
-  <si>
-    <t>arquivo excel BW</t>
   </si>
   <si>
     <t>BR_PRODUCT.txt
@@ -262,12 +259,31 @@
   <si>
     <t>IEAZIWSQLD001 (10.63.252.71)</t>
   </si>
+  <si>
+    <t xml:space="preserve">BRSPIIS01
+FRIAPFIL03
+</t>
+  </si>
+  <si>
+    <t>FRIAPSQLGL02</t>
+  </si>
+  <si>
+    <t>base_externa.txt
+base_externa_real.txt
+Consumo – AC.csv , Consumo - DN.csv, Consumo -  DS.csv , Consumo-  KS.csv, Consumo – VI.csv
+Vendas – AC.csv , Vendas - DN.csv, Vendas -  DS.csv , Vendas -  KS.csv, Vendas – VI.csv
+base_externa.txt
+movimentação.txt
+ajustes_TeamSpace-SIP.xlsx, ajustes_TeamSpace-LIFE.xlsx e ajustes_TeamSpace-SPIFF.xlsx
+Ajustes_Auditoria_SIP.CSV, Ajustes_Auditoria_SPIFF.CSV, e Ajustes_Auditoria_LIFE.CSV
+base_externa_REAL-KPI_LIFE.csv, base_externa_REAL-KPI_SIP.csv, e base_externa_REAL-KPI_SPIFF.csv</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +319,13 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -379,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -418,6 +441,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -704,9 +733,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +916,7 @@
         <v>51</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -930,19 +959,19 @@
         <v>147167169205</v>
       </c>
       <c r="E9" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
@@ -964,8 +993,8 @@
       <c r="G10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>65</v>
+      <c r="H10" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -990,9 +1019,7 @@
       <c r="G11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>65</v>
-      </c>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1016,9 +1043,7 @@
       <c r="G12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>65</v>
-      </c>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1081,10 +1106,10 @@
         <v>11</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>56</v>
@@ -1143,7 +1168,7 @@
         <v>55</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1220,7 +1245,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1236,11 +1261,11 @@
       <c r="E21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>22</v>
+      <c r="F21" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="H21" s="13"/>
     </row>

</xml_diff>